<commit_message>
Fixed bugs and added RTM
</commit_message>
<xml_diff>
--- a/Lesson_2/Cooler_Requirements_Panchenko_Andrey.xlsx
+++ b/Lesson_2/Cooler_Requirements_Panchenko_Andrey.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrey\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FB98E5-004F-4EFF-8960-0D5A64F59CC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B72593-A822-4C41-8F0F-9D351022CA46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{10141C68-1F09-40E0-A98A-1B910715773E}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="Traceability" sheetId="2" r:id="rId2"/>
+    <sheet name="RTM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
   <si>
     <t>Правильность</t>
   </si>
@@ -118,9 +118,6 @@
 describes what should be at the bottom of the cooler case</t>
   </si>
   <si>
-    <t>Place the cooling and water heating buttons on the top of the back of the cooler. Below the condenser, the hot water drain valve, and even below the power cord.</t>
-  </si>
-  <si>
     <t>+
 describes exactly what should be on the back of the cooler</t>
   </si>
@@ -135,15 +132,6 @@
     <t>Requirements</t>
   </si>
   <si>
-    <t>Install the glass dispenser</t>
-  </si>
-  <si>
-    <t>Measure the temperature after heating. Measure the temperature before the second heating.</t>
-  </si>
-  <si>
-    <t>Read instructions</t>
-  </si>
-  <si>
     <t>The cooler should stand well on the surface. Have adjustable feet for greater stability on bumps.</t>
   </si>
   <si>
@@ -157,19 +145,118 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Inspect the front side of the cooler</t>
-  </si>
-  <si>
-    <t>Place glasses in storage space</t>
-  </si>
-  <si>
-    <t>Inspect the back of the cooler</t>
-  </si>
-  <si>
     <t>Check cooler operation at voltage from 115 to 120 volts</t>
   </si>
   <si>
-    <t>Place the cooler on an uneven surface and, by adjusting the legs, make it stand level</t>
+    <t>Check the installation of the glass dispenser on the cooler.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check if the holes for the cup dispenser are made in the upper part of the right side panel of the cooler </t>
+  </si>
+  <si>
+    <t>Check that the dispenser holes on the cooler are covered with a plastic cover</t>
+  </si>
+  <si>
+    <t>Check the temperature after heating the water in the cooler</t>
+  </si>
+  <si>
+    <t>Check if the heating indicator is red when heating water in the cooler</t>
+  </si>
+  <si>
+    <t>Check how long it takes to heat water in a cooler</t>
+  </si>
+  <si>
+    <t>Check at what temperature the water in the cooler starts to heat up again</t>
+  </si>
+  <si>
+    <t>Check if the cycle of heating the water in the cooler repeats after it cools down</t>
+  </si>
+  <si>
+    <t>Check if the heating indicator goes out when the water temperature in the cooler reaches 90ºC</t>
+  </si>
+  <si>
+    <t>Check if the cooler is in power saving mode</t>
+  </si>
+  <si>
+    <t>Check if the water in the cooler heats up to 60ºC in the energy saving mode</t>
+  </si>
+  <si>
+    <t>Check if the water heating indicator on the cooler is on when water is heated in energy saving mode in red</t>
+  </si>
+  <si>
+    <t>Check if the water heating indicator on the cooler goes out when the water in energy saving mode reaches 60ºC</t>
+  </si>
+  <si>
+    <t>Check how much time it takes to heat water in a cooler in energy saving mode</t>
+  </si>
+  <si>
+    <t>Check if the power saving mode affects the water cooling in the cooler</t>
+  </si>
+  <si>
+    <t>Check the water temperature in the cooler after cooling</t>
+  </si>
+  <si>
+    <t>Check if the water cooling indicator on the cooler is blue when the water is being cooled</t>
+  </si>
+  <si>
+    <t>Check if the water cooling indicator on the cooler goes out when the water temperature reaches 7 ℃</t>
+  </si>
+  <si>
+    <t>Check at what temperature the water in the cooler starts to cool again</t>
+  </si>
+  <si>
+    <t>Check if the water cooling cycle in the cooler repeats after it heats up</t>
+  </si>
+  <si>
+    <t>Check the instructions for the cooler for spelling errors</t>
+  </si>
+  <si>
+    <t>Check the instructions for the cooler for the presence of cooler characteristics</t>
+  </si>
+  <si>
+    <t>Check if the instructions for the cooler are clear to the user</t>
+  </si>
+  <si>
+    <t>Check the front side of the cooler for the presence of an electronic LED display and control panel.</t>
+  </si>
+  <si>
+    <t>Check the location of the valves on the front side of the cooler</t>
+  </si>
+  <si>
+    <t>Check if the screen, taps, indicators on the front panel of the cooler are working correctly</t>
+  </si>
+  <si>
+    <t>Check the cooler for storage space</t>
+  </si>
+  <si>
+    <t>Check the storage space in the cooler for the capacity of the glasses</t>
+  </si>
+  <si>
+    <t>Check the back of the cooler for buttons for heating and cooling water</t>
+  </si>
+  <si>
+    <t>Check if the buttons on the back of the cooler work</t>
+  </si>
+  <si>
+    <t>Check the operation of the hot water drain tap on the cooler</t>
+  </si>
+  <si>
+    <t>Place the cooling and water heating buttons at the top of the back of the cooler. Below is a condenser, under it is a hot water drain tap, a power cord.</t>
+  </si>
+  <si>
+    <t>Check if the cooler will work at a higher or lower voltage than the recommended</t>
+  </si>
+  <si>
+    <t>Check if the cooler will be through an adapter or extension</t>
+  </si>
+  <si>
+    <t>Check if the cooler is well placed on a flat surface</t>
+  </si>
+  <si>
+    <t>Check if you can put the cooler on an uneven surface by adjusting the legs</t>
+  </si>
+  <si>
+    <t>Check if the feet adjustment works on the cooler</t>
   </si>
 </sst>
 </file>
@@ -227,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -250,11 +337,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -290,7 +414,22 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,7 +748,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +918,7 @@
     </row>
     <row r="8" spans="1:7" ht="141" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>24</v>
@@ -802,10 +941,10 @@
     </row>
     <row r="9" spans="1:7" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>6</v>
@@ -825,10 +964,10 @@
     </row>
     <row r="10" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>6</v>
@@ -848,10 +987,10 @@
     </row>
     <row r="11" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>6</v>
@@ -877,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D78E734-4108-48DF-BDF7-B4E4FB75E7F5}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,10 +1037,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -909,79 +1048,231 @@
         <v>11</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="147" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A3" s="13"/>
       <c r="B3" s="11" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A4" s="14"/>
       <c r="B4" s="11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B16" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B18" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B21" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B22" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B25" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B28" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="63" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="B30" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B31" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B33" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B34" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>41</v>
+    </row>
+    <row r="36" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B36" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B37" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B39" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B40" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>